<commit_message>
select credential type to run
</commit_message>
<xml_diff>
--- a/configuration.xlsx
+++ b/configuration.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569AA0A7-F3CC-4FE5-8B46-AD9CEE6A6C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02163A45-3A4B-4E48-9037-5F94CA056E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="2715" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="176">
   <si>
     <t>key</t>
   </si>
@@ -551,6 +551,12 @@
   </si>
   <si>
     <t>2475448649908224000</t>
+  </si>
+  <si>
+    <t>CREDENTIAL_TYPE</t>
+  </si>
+  <si>
+    <t>window</t>
   </si>
 </sst>
 </file>
@@ -652,7 +658,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -703,6 +709,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -908,8 +920,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C6DC0DE-EED2-4CDC-897B-F346060614D6}" name="Tabla1" displayName="Tabla1" ref="A1:E73" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A1:E73" xr:uid="{1C6DC0DE-EED2-4CDC-897B-F346060614D6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C6DC0DE-EED2-4CDC-897B-F346060614D6}" name="Tabla1" displayName="Tabla1" ref="A1:E74" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:E74" xr:uid="{1C6DC0DE-EED2-4CDC-897B-F346060614D6}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{5459FF77-70C5-4191-86A3-14F8988CB3AA}" name="key" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{A6896349-98DD-46FD-9311-0EE1C19B4B3E}" name="env" dataDxfId="3"/>
@@ -1191,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1491,43 +1503,37 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>90</v>
-      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="3">
-        <v>10</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>52</v>
+        <v>73</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1535,10 +1541,10 @@
         <v>54</v>
       </c>
       <c r="B25" s="3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>22</v>
@@ -1549,242 +1555,242 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>155</v>
+        <v>54</v>
+      </c>
+      <c r="B26" s="3">
+        <v>30</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>155</v>
+        <v>51</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C28" s="10" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>163</v>
-      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C33" s="10"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
+      <c r="C34" s="10"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>173</v>
-      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C36" s="16">
-        <v>-804214108</v>
+        <v>172</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
+      </c>
+      <c r="C37" s="16">
+        <v>-804214108</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>59</v>
+        <v>169</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>18</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>131</v>
-      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E44" s="3" t="s">
+      <c r="D45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
+    <row r="46" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C46" s="11">
         <v>3</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="E46" s="15" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B48" s="3">
-        <v>10</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>153</v>
+        <v>124</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1792,16 +1798,16 @@
         <v>143</v>
       </c>
       <c r="B49" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1809,7 +1815,7 @@
         <v>143</v>
       </c>
       <c r="B50" s="3">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C50" s="14" t="s">
         <v>127</v>
@@ -1822,146 +1828,149 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B51" s="3">
+        <v>30</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>114</v>
-      </c>
+      <c r="B52" s="7"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>140</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E54" s="4" t="s">
-        <v>96</v>
+      <c r="E54" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>99</v>
+        <v>30</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>100</v>
+      <c r="E57" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C59" s="11">
-        <v>587</v>
+        <v>62</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
+      </c>
+      <c r="C60" s="11">
+        <v>587</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>22</v>
@@ -1972,94 +1981,94 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>56</v>
+        <v>64</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>36</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C67" s="13" t="s">
-        <v>77</v>
+        <v>33</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>22</v>
@@ -2070,10 +2079,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>22</v>
@@ -2084,49 +2093,68 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E70" s="3" t="s">
+      <c r="D71" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E73" s="3" t="s">
+      <c r="D74" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74" s="3" t="s">
         <v>142</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22" xr:uid="{CB8A3CD4-7BE5-4025-B439-28867B8E0C53}">
+      <formula1>"window,asset"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -2136,9 +2164,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2326,19 +2357,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79E76BC6-FD13-4E9A-B822-542E612CA8CB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1650C86-818B-4C5F-85BF-D8BB24902BFD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2362,9 +2389,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1650C86-818B-4C5F-85BF-D8BB24902BFD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79E76BC6-FD13-4E9A-B822-542E612CA8CB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update google sheet chua xong
</commit_message>
<xml_diff>
--- a/configuration.xlsx
+++ b/configuration.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02163A45-3A4B-4E48-9037-5F94CA056E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5639711-61D5-4D37-B777-48D8A4808C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="178">
   <si>
     <t>key</t>
   </si>
@@ -442,9 +442,6 @@
   </si>
   <si>
     <t>Default: True. Replace all paths containing user with the session user.</t>
-  </si>
-  <si>
-    <t>3_state</t>
   </si>
   <si>
     <t>Strongly suggested value: Daily: 15, Monthly: 3, Yearly: 2, standalone: 1. 
@@ -557,6 +554,15 @@
   </si>
   <si>
     <t>window</t>
+  </si>
+  <si>
+    <t>3_consolidate</t>
+  </si>
+  <si>
+    <t>GSHEET_KEY_FILE</t>
+  </si>
+  <si>
+    <t>1tG4lp6N0xVe_uVqvtfKhXxXLPBNg17tWgspPisvevPk</t>
   </si>
 </sst>
 </file>
@@ -658,7 +664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -709,12 +715,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -920,8 +920,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C6DC0DE-EED2-4CDC-897B-F346060614D6}" name="Tabla1" displayName="Tabla1" ref="A1:E74" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A1:E74" xr:uid="{1C6DC0DE-EED2-4CDC-897B-F346060614D6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C6DC0DE-EED2-4CDC-897B-F346060614D6}" name="Tabla1" displayName="Tabla1" ref="A1:E76" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:E76" xr:uid="{1C6DC0DE-EED2-4CDC-897B-F346060614D6}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{5459FF77-70C5-4191-86A3-14F8988CB3AA}" name="key" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{A6896349-98DD-46FD-9311-0EE1C19B4B3E}" name="env" dataDxfId="3"/>
@@ -1203,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1242,7 +1242,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>22</v>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>24</v>
@@ -1394,10 +1394,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1405,7 +1405,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>24</v>
@@ -1439,7 +1439,7 @@
         <v>21</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.3">
@@ -1496,22 +1496,19 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>161</v>
-      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
@@ -1527,7 +1524,7 @@
         <v>73</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>18</v>
@@ -1572,18 +1569,18 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>156</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1597,31 +1594,31 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
@@ -1629,474 +1626,457 @@
       <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C34" s="10"/>
+      <c r="A34" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
+      <c r="C35" s="10"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>173</v>
-      </c>
+      <c r="C36" s="10"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C37" s="16">
-        <v>-804214108</v>
-      </c>
+      <c r="A37" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>18</v>
+        <v>167</v>
+      </c>
+      <c r="C39" s="16">
+        <v>-804214108</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>60</v>
+        <v>168</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>57</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
+      <c r="A42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>128</v>
+        <v>58</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>131</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>134</v>
-      </c>
+      <c r="A44" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C46" s="11">
-        <v>3</v>
+        <v>132</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>139</v>
+        <v>22</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
+      </c>
+      <c r="C48" s="11">
+        <v>3</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>125</v>
+        <v>21</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="B49" s="3">
-        <v>10</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B50" s="3">
-        <v>20</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>127</v>
+        <v>124</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B51" s="3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
+      <c r="A52" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" s="3">
+        <v>20</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>140</v>
+        <v>142</v>
+      </c>
+      <c r="B53" s="3">
+        <v>30</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>127</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>67</v>
-      </c>
+      <c r="A54" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" s="7"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>93</v>
+        <v>15</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>139</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E55" s="4" t="s">
-        <v>96</v>
+      <c r="E55" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E56" s="4" t="s">
-        <v>97</v>
+      <c r="E56" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>99</v>
+        <v>29</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>100</v>
+      <c r="E58" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>113</v>
+        <v>30</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E59" s="3" t="s">
-        <v>83</v>
+      <c r="E59" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C60" s="11">
-        <v>587</v>
+        <v>61</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>148</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
+      </c>
+      <c r="C62" s="11">
+        <v>587</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>36</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>47</v>
+        <v>64</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>41</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C68" s="13" t="s">
-        <v>77</v>
+        <v>34</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>82</v>
+        <v>33</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>22</v>
@@ -2107,46 +2087,74 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E71" s="3" t="s">
+      <c r="D73" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>142</v>
+      <c r="D76" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update giờ vào việc, giờ tan làm vào config
</commit_message>
<xml_diff>
--- a/configuration.xlsx
+++ b/configuration.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5639711-61D5-4D37-B777-48D8A4808C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="184">
   <si>
     <t>key</t>
   </si>
@@ -553,9 +552,6 @@
     <t>CREDENTIAL_TYPE</t>
   </si>
   <si>
-    <t>window</t>
-  </si>
-  <si>
     <t>3_consolidate</t>
   </si>
   <si>
@@ -563,13 +559,34 @@
   </si>
   <si>
     <t>1tG4lp6N0xVe_uVqvtfKhXxXLPBNg17tWgspPisvevPk</t>
+  </si>
+  <si>
+    <t>asset</t>
+  </si>
+  <si>
+    <t>TIME_CHECK_IN</t>
+  </si>
+  <si>
+    <t>TIME_CHECK_OUT</t>
+  </si>
+  <si>
+    <t>LAST_TIME_CHECK_OUT</t>
+  </si>
+  <si>
+    <t>giờ tan làm ngày thứ 7</t>
+  </si>
+  <si>
+    <t>tan làm ngày bình thường</t>
+  </si>
+  <si>
+    <t>giờ vào làm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,6 +653,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Open Sans"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -664,7 +687,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -715,6 +738,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -735,7 +767,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Open Sans"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -760,7 +791,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Open Sans"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -785,7 +815,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Open Sans"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -810,7 +839,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Open Sans"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -829,7 +857,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Open Sans"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -870,7 +897,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Open Sans"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -895,7 +921,6 @@
         <sz val="11"/>
         <color theme="0"/>
         <name val="Open Sans"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -920,14 +945,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C6DC0DE-EED2-4CDC-897B-F346060614D6}" name="Tabla1" displayName="Tabla1" ref="A1:E76" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A1:E76" xr:uid="{1C6DC0DE-EED2-4CDC-897B-F346060614D6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E79" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:E79"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5459FF77-70C5-4191-86A3-14F8988CB3AA}" name="key" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{A6896349-98DD-46FD-9311-0EE1C19B4B3E}" name="env" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{BA781C67-D08F-467D-A16D-C1307CBCBFA5}" name="value" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{61BF72FF-CA4C-48C2-9848-3FF18BEAB94C}" name="item_class" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{DA443A43-83AE-4C11-879F-A559B611CEC4}" name="description" dataDxfId="0"/>
+    <tableColumn id="1" name="key" dataDxfId="4"/>
+    <tableColumn id="5" name="env" dataDxfId="3"/>
+    <tableColumn id="2" name="value" dataDxfId="2"/>
+    <tableColumn id="3" name="item_class" dataDxfId="1"/>
+    <tableColumn id="4" name="description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1202,25 +1227,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="30.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.69921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.796875" style="3" customWidth="1"/>
     <col min="4" max="4" width="14" style="3" customWidth="1"/>
-    <col min="5" max="5" width="68.33203125" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.77734375" style="3"/>
+    <col min="5" max="5" width="68.296875" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1237,7 +1262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1251,7 +1276,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1265,7 +1290,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1279,7 +1304,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1293,7 +1318,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>87</v>
       </c>
@@ -1307,7 +1332,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>40</v>
       </c>
@@ -1321,7 +1346,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1335,7 +1360,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
@@ -1350,7 +1375,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
         <v>136</v>
       </c>
@@ -1364,7 +1389,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1378,7 +1403,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1392,7 +1417,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
         <v>157</v>
       </c>
@@ -1400,7 +1425,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
@@ -1414,7 +1439,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
         <v>115</v>
       </c>
@@ -1428,7 +1453,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -1442,7 +1467,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="15.6">
       <c r="A17" s="5" t="s">
         <v>10</v>
       </c>
@@ -1457,7 +1482,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
@@ -1466,7 +1491,7 @@
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -1480,7 +1505,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
@@ -1494,7 +1519,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
         <v>159</v>
       </c>
@@ -1502,15 +1527,15 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
         <v>173</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>110</v>
       </c>
@@ -1519,7 +1544,7 @@
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
         <v>73</v>
       </c>
@@ -1533,7 +1558,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
         <v>54</v>
       </c>
@@ -1550,7 +1575,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
@@ -1567,7 +1592,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
         <v>154</v>
       </c>
@@ -1575,7 +1600,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
         <v>155</v>
       </c>
@@ -1583,7 +1608,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
         <v>111</v>
       </c>
@@ -1592,7 +1617,7 @@
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
         <v>161</v>
       </c>
@@ -1600,7 +1625,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
         <v>163</v>
       </c>
@@ -1608,7 +1633,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
         <v>165</v>
       </c>
@@ -1616,550 +1641,589 @@
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
+    <row r="33" spans="1:5">
+      <c r="A33" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" s="20">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B35" s="19"/>
+      <c r="C35" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="C37" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C35" s="10"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C36" s="10"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
+    </row>
+    <row r="38" spans="1:5">
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C41" s="17" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
+    <row r="42" spans="1:5">
+      <c r="A42" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C39" s="16">
+      <c r="C42" s="16">
         <v>-804214108</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
+    <row r="43" spans="1:5">
+      <c r="A43" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
+    <row r="44" spans="1:5">
+      <c r="A44" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+    <row r="45" spans="1:5">
+      <c r="A45" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
+    <row r="46" spans="1:5">
+      <c r="A46" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
+    <row r="47" spans="1:5">
+      <c r="A47" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
+      <c r="B47" s="7"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
+    <row r="49" spans="1:5">
+      <c r="A49" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="D49" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
+    <row r="50" spans="1:5">
+      <c r="A50" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E47" s="3" t="s">
+      <c r="D50" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
+    <row r="51" spans="1:5" ht="27.6">
+      <c r="A51" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C48" s="11">
+      <c r="C51" s="11">
         <v>3</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E48" s="15" t="s">
+      <c r="E51" s="15" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
+    <row r="52" spans="1:5">
+      <c r="A52" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E52" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
+    <row r="53" spans="1:5">
+      <c r="A53" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
+    <row r="54" spans="1:5">
+      <c r="A54" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B54" s="3">
         <v>10</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C54" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
+    <row r="55" spans="1:5">
+      <c r="A55" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B55" s="3">
         <v>20</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C55" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E55" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
+    <row r="56" spans="1:5">
+      <c r="A56" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B56" s="3">
         <v>30</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C56" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
+    <row r="57" spans="1:5">
+      <c r="A57" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
+      <c r="B57" s="7"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C58" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E55" s="3" t="s">
+      <c r="D58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
+    <row r="59" spans="1:5">
+      <c r="A59" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C59" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E56" s="3" t="s">
+      <c r="D59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
+    <row r="60" spans="1:5">
+      <c r="A60" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C60" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E57" s="4" t="s">
+      <c r="D60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
+    <row r="61" spans="1:5">
+      <c r="A61" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C61" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E58" s="4" t="s">
+      <c r="D61" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
+    <row r="62" spans="1:5">
+      <c r="A62" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C62" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E59" s="4" t="s">
+      <c r="D62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
+    <row r="63" spans="1:5">
+      <c r="A63" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E60" s="3" t="s">
+      <c r="D63" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
+    <row r="64" spans="1:5">
+      <c r="A64" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E61" s="3" t="s">
+      <c r="D64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
+    <row r="65" spans="1:5">
+      <c r="A65" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C62" s="11">
+      <c r="C65" s="11">
         <v>587</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E65" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
+    <row r="66" spans="1:5">
+      <c r="A66" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E63" s="3" t="s">
+      <c r="D66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
+    <row r="67" spans="1:5">
+      <c r="A67" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E64" s="3" t="s">
+      <c r="D67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
+    <row r="68" spans="1:5">
+      <c r="A68" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C68" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E69" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
+    <row r="73" spans="1:5">
+      <c r="A73" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C70" s="13" t="s">
+      <c r="C73" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E70" s="3" t="s">
+      <c r="D73" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="3" t="s">
+    <row r="74" spans="1:5">
+      <c r="A74" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C74" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E71" s="3" t="s">
+      <c r="D74" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
+    <row r="75" spans="1:5">
+      <c r="A75" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C75" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E72" s="3" t="s">
+      <c r="D75" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E75" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
+    <row r="76" spans="1:5">
+      <c r="A76" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E73" s="3" t="s">
+      <c r="D76" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="3" t="s">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A77" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E74" s="3" t="s">
+      <c r="D77" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A78" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D75" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E75" s="3" t="s">
+      <c r="D78" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A79" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D76" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E76" s="3" t="s">
+      <c r="D79" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>141</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22" xr:uid="{CB8A3CD4-7BE5-4025-B439-28867B8E0C53}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22">
       <formula1>"window,asset"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>